<commit_message>
feat: Final modification on scrum schedule (task6-scrum-setup)
</commit_message>
<xml_diff>
--- a/doc/task6/scrum_task06_Orange_v2.xlsx
+++ b/doc/task6/scrum_task06_Orange_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yannis/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yannis/IntelliJProjects/SoED/ch.bfh.bti7081.s2019.orange/doc/task6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28290FF2-072C-8D45-99D4-80BC2FCB0728}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A8304F-1C8A-C14C-9137-6E234AF10F57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="110">
   <si>
     <t>ID</t>
   </si>
@@ -215,16 +215,6 @@
   </si>
   <si>
     <t>Die im  Klassendiagramm definierten Klassen sind zu implementieren. Zur Zeit noch ohne Logik, jedoch mit den nötigen Attributen sowie getter und setter Methoden.</t>
-  </si>
-  <si>
-    <t>Evaluation JSON Library</t>
-  </si>
-  <si>
-    <t>Es ist eine JSON-Library zu evaluieren, die es ermöglicht mittles Java JSON-Files zu parsen.
-(Evt. GSON)</t>
-  </si>
-  <si>
-    <t>JSON Parser PoC</t>
   </si>
   <si>
     <t xml:space="preserve">Die CRUD Funktionen müssen demonstriert werden können.
@@ -241,47 +231,10 @@
     <t>Testdaten erstellen</t>
   </si>
   <si>
-    <t xml:space="preserve">Es sollen JSON plaintext Daten erstellt werden.
-Mindestens zwei Ärzte sowie ein Patient mite einem Dossiert, welches ein Report beinhaltet.
-</t>
-  </si>
-  <si>
-    <t>Struktur der JSON Daten definieren</t>
-  </si>
-  <si>
-    <t>Die Striktur der Testdaten soll definiert werden.
-(Ärzte, Dossiert, Reports (Messages?))</t>
-  </si>
-  <si>
     <t>Ärzte Auswahl</t>
   </si>
   <si>
-    <t>Patienten Auswahl</t>
-  </si>
-  <si>
-    <t>Anhand des ausgewälten Arztes, sollen alle seine  Patienten aufgelistet werden.</t>
-  </si>
-  <si>
-    <t>Als initiale WebPage soll eine Liste aller erfassten Ärzten angezeigt werden.  Dabei soll der Arzt ausgewält werden, als welchen man das Tool verwenden will.
-Die Auswahl des Arztes (button-click) führt also zur nächsten View.</t>
-  </si>
-  <si>
-    <t>Auswahl der Reports</t>
-  </si>
-  <si>
-    <t>Nach der Auswahl des Patienten sollen alle dazugehörigen Reports aufgelistet werden.</t>
-  </si>
-  <si>
     <t>Anzeig Report</t>
-  </si>
-  <si>
-    <t>Anzeig des Reports und Platzhalter für Nachrichten. Die Eingabefelder sind lediglich MockUp</t>
-  </si>
-  <si>
-    <t>JSON Parser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mittels  JSON Parser soll aus JSON Files Objekte, der in Punkt 8.1 definierten Klassen, erstellt werden. </t>
   </si>
   <si>
     <t>Auseinandersetzen mit dem Technologie Stack</t>
@@ -309,9 +262,6 @@
     <t>Lars Peyer</t>
   </si>
   <si>
-    <t>Mathias Ossola</t>
-  </si>
-  <si>
     <t>Sub-ID</t>
   </si>
   <si>
@@ -349,6 +299,83 @@
   </si>
   <si>
     <t>Verbleibende Ressourcen</t>
+  </si>
+  <si>
+    <t>Anzeige Dossiers (Patienten Auswahl)</t>
+  </si>
+  <si>
+    <t>Detailansicht Dossier
+(Auswahl der Reports)</t>
+  </si>
+  <si>
+    <t>MongoDB PoC</t>
+  </si>
+  <si>
+    <t>MongoDB Installation auf Windows</t>
+  </si>
+  <si>
+    <t>UnitOfWork Klasse implementieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Di UnitOfWork-Klasse soll implementiert werden, die die Verbinung zur mongoDB ermöglicht. Ebenfalls soll diese die CRUD Funktionalitäten für Patienten, Ärzte und Report Repositories zur Verfügung stellen.
+</t>
+  </si>
+  <si>
+    <t>Als initiale WebPage soll eine Liste aller erfassten Ärzten angezeigt werden.  Dabei soll der Arzt ausgewält werden, als welchen man das Tool verwenden will.
+Die Auswahl des Arztes (button-click) führt also zur nächsten View.
+Die Daten sind vorerst Hard-Coded.</t>
+  </si>
+  <si>
+    <t>Anhand des ausgewälten Arztes, sollen alle seine  Patienten bzw. dessen Dossiers aufgelistet werden.
+Die Auswahl eines Dossiers führt zur nächsten View.
+Die Daten sind vorerst Hard-Coded.</t>
+  </si>
+  <si>
+    <t>Nach der Auswahl des Patienten-Dossier sollen dessen Daten sowie alle dazugehörigen Reports aufgelistet werden.
+Die Daten sind vorerst Hard-Coded.</t>
+  </si>
+  <si>
+    <t>Anzeig des Reports und Platzhalter für Nachrichten. Die Eingabefelder sind lediglich MockUp.
+Die Daten sind vorerst Hard-Coded.</t>
+  </si>
+  <si>
+    <t>Ärzte Auswahl mit Testdaten</t>
+  </si>
+  <si>
+    <t>Die Daten der angezeigten  Ärzten sollen aus der DB entnommen werden.</t>
+  </si>
+  <si>
+    <t>Die Daten der angezeigten  Dossiers sollen aus der DB entnommen werden.</t>
+  </si>
+  <si>
+    <t>Die Daten des Inhalts  der angezeigten  Dossiers sollen aus der DB entnommen werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Es soll ein Skript erstellt werden, welches die Datenbank bereinigt und mit initialen Testdaten füttert
+Diese sollen mindestens zwei Ärzte sowie ein Patient mit einem Dossiert, welches ein Report beinhaltet aufweisen.
+</t>
+  </si>
+  <si>
+    <t>Anzeige Dossiers mit Testdaten</t>
+  </si>
+  <si>
+    <t>Anzeige Detailansicht mit Testdaten</t>
+  </si>
+  <si>
+    <t>Anzeige Report mit Testdaten</t>
+  </si>
+  <si>
+    <t>Die Daten des Inhalts  der angezeigten  Reports sollen aus der DB entnommen werden.</t>
+  </si>
+  <si>
+    <t>Anleitung zur Installation und Verwendung der MongoDB auf Windows</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -453,7 +480,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -708,11 +735,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -737,9 +875,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -747,38 +882,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -790,6 +907,90 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,42 +1000,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -844,41 +1009,56 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -886,6 +1066,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -916,16 +1116,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1265,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1297,7 +1487,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -1313,7 +1503,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -1321,7 +1511,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -1329,7 +1519,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
@@ -1347,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A3" zoomScale="99" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1390,339 +1580,365 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.2">
-      <c r="A2" s="28">
+      <c r="A2" s="21">
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="E2" s="12">
+        <v>35</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="96" x14ac:dyDescent="0.2">
-      <c r="A3" s="28">
+      <c r="A3" s="21">
         <f t="shared" ref="A3:A14" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="E3" s="12">
+        <v>50</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A4" s="28">
+      <c r="A4" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="E4" s="12">
+        <v>20</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="28">
+      <c r="A5" s="21">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="14" t="s">
+      <c r="E5" s="12">
+        <v>100</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="28">
+      <c r="A6" s="21">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="14" t="s">
+      <c r="E6" s="12">
+        <v>50</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="28">
+      <c r="A7" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="14" t="s">
+      <c r="E7" s="12">
+        <v>80</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="28">
+      <c r="A8" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="14" t="s">
+      <c r="E8" s="12">
+        <v>6</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="28">
+      <c r="A9" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="14" t="s">
+      <c r="E9" s="12">
+        <v>16</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="28">
+      <c r="A10" s="21">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="14" t="s">
+      <c r="E10" s="12">
+        <v>4</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="28">
+      <c r="A11" s="21">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="14" t="s">
+      <c r="E11" s="12">
+        <v>50</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="28">
+      <c r="A12" s="21">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="14" t="s">
+      <c r="E12" s="12">
+        <v>15</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="28">
+      <c r="A13" s="21">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="14" t="s">
+      <c r="E13" s="12">
+        <v>30</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="28">
+      <c r="A14" s="21">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="14" t="s">
+      <c r="E14" s="12">
+        <v>20</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="9"/>
@@ -2373,10 +2589,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2401,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>11</v>
@@ -2438,443 +2655,440 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
+      <c r="A2" s="44">
         <v>0</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="13">
         <v>0</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="D2" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="16">
-        <v>2</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" s="19" t="s">
+      <c r="J2" s="13">
+        <v>1</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
-      <c r="B3" s="12">
+      <c r="A3" s="45"/>
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="12">
-        <v>2</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3" s="21" t="s">
+      <c r="J3" s="11">
+        <v>1</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="12">
+      <c r="A4" s="45"/>
+      <c r="B4" s="11">
         <v>0</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="12" t="s">
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="12">
-        <v>2</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M4" s="21" t="s">
+      <c r="J4" s="11">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="12">
+      <c r="A5" s="45"/>
+      <c r="B5" s="11">
         <v>0</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="12" t="s">
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="12">
-        <v>2</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="21" t="s">
+      <c r="J5" s="11">
+        <v>1</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="12">
+      <c r="A6" s="45"/>
+      <c r="B6" s="11">
         <v>0</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>1</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="12" t="s">
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="12">
-        <v>2</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M6" s="21" t="s">
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23">
+      <c r="A7" s="46"/>
+      <c r="B7" s="17">
         <v>0</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="17">
         <v>1</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="23" t="s">
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="23">
-        <v>2</v>
-      </c>
-      <c r="K7" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="L7" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="M7" s="26" t="s">
+      <c r="J7" s="17">
+        <v>1</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="27"/>
+      <c r="Q7" s="20"/>
     </row>
     <row r="8" spans="1:18" ht="128" x14ac:dyDescent="0.2">
-      <c r="A8" s="29">
+      <c r="A8" s="50">
         <f>'Product Backlog'!A9</f>
         <v>8</v>
       </c>
-      <c r="B8" s="18" t="str">
+      <c r="B8" s="14" t="str">
         <f>_xlfn.CONCAT(A8, ".",ROW(A8)-ROW()+1)</f>
         <v>8.1</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <v>1</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="14">
+        <v>2</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" s="10"/>
+    </row>
+    <row r="9" spans="1:18" ht="96" x14ac:dyDescent="0.2">
+      <c r="A9" s="51"/>
+      <c r="B9" s="12">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="12">
+        <v>4</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="12">
+        <v>4</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="176" x14ac:dyDescent="0.2">
+      <c r="A10" s="51"/>
+      <c r="B10" s="12">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="12">
+        <v>4</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
+      <c r="B11" s="18">
+        <v>8.4</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="18">
+        <v>4</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A12" s="60"/>
+      <c r="B12" s="61">
+        <v>7.1</v>
+      </c>
+      <c r="C12" s="61">
+        <v>1</v>
+      </c>
+      <c r="D12" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="E12" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="18">
+      <c r="H12" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="61">
         <v>2</v>
       </c>
-      <c r="K8" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="M8" s="19" t="s">
+      <c r="K12" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="R8" s="11"/>
-    </row>
-    <row r="9" spans="1:18" ht="80" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="14">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="C9" s="14">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" s="14">
-        <v>2</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M9" s="21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="96" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="14">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="C10" s="14">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="14">
-        <v>4</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L10" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M10" s="21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="80" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="14">
-        <v>8.4</v>
-      </c>
-      <c r="C11" s="14">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="14">
-        <v>4</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M11" s="21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="25">
-        <v>8.5</v>
-      </c>
-      <c r="C12" s="25">
-        <v>1</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" s="25">
-        <v>4</v>
-      </c>
-      <c r="K12" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="L12" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="M12" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="80" x14ac:dyDescent="0.2">
-      <c r="A13" s="15">
-        <f>'Product Backlog'!A8</f>
-        <v>7</v>
-      </c>
+    </row>
+    <row r="13" spans="1:18" ht="209" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="46"/>
       <c r="B13" s="18">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="C13" s="18">
         <v>1</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E13" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>87</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="16" t="s">
-        <v>5</v>
+      <c r="I13" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="J13" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>58</v>
@@ -2886,247 +3100,322 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25">
-        <v>7.2</v>
-      </c>
-      <c r="C14" s="25">
-        <v>1</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="25">
-        <v>2</v>
-      </c>
-      <c r="K14" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="L14" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="M14" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="176" x14ac:dyDescent="0.2">
-      <c r="A15" s="15">
+    <row r="14" spans="1:18" ht="208" x14ac:dyDescent="0.2">
+      <c r="A14" s="44">
         <f>'Product Backlog'!A3</f>
         <v>2</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B14" s="14">
         <v>2.1</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C14" s="14">
         <v>1</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="D14" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="14">
+        <v>4</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A15" s="64"/>
+      <c r="B15" s="65">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C15" s="65">
+        <v>1</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="65">
+        <v>4</v>
+      </c>
+      <c r="K15" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" s="67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="176" x14ac:dyDescent="0.2">
+      <c r="A16" s="45"/>
+      <c r="B16" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="12">
+        <v>4</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="45"/>
+      <c r="B17" s="12">
+        <v>2.4</v>
+      </c>
+      <c r="C17" s="12">
+        <v>1</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="12">
+        <v>4</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="128" x14ac:dyDescent="0.2">
+      <c r="A18" s="45"/>
+      <c r="B18" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="I15" s="16" t="s">
+      <c r="H18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J18" s="12">
         <v>4</v>
       </c>
-      <c r="K15" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="L15" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="M15" s="19" t="s">
+      <c r="K18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="80" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="14">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C16" s="14">
+    <row r="19" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="A19" s="68"/>
+      <c r="B19" s="57">
+        <v>2.6</v>
+      </c>
+      <c r="C19" s="57">
         <v>1</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="I16" s="12" t="s">
+      <c r="D19" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="57">
+        <v>4</v>
+      </c>
+      <c r="K19" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="M19" s="59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="68"/>
+      <c r="B20" s="18">
+        <v>2.7</v>
+      </c>
+      <c r="C20" s="18">
+        <v>1</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J20" s="18">
         <v>4</v>
       </c>
-      <c r="K16" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M16" s="21" t="s">
+      <c r="K20" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M20" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="64" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="14">
-        <v>2.4</v>
-      </c>
-      <c r="C17" s="14">
+    <row r="21" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="46"/>
+      <c r="B21" s="18">
+        <v>2.8</v>
+      </c>
+      <c r="C21" s="18">
         <v>1</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="14">
+      <c r="D21" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="18">
         <v>4</v>
       </c>
-      <c r="K17" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="L17" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M17" s="21" t="s">
+      <c r="K21" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M21" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="25">
-        <v>2.5</v>
-      </c>
-      <c r="C18" s="25">
-        <v>1</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="25">
-        <v>4</v>
-      </c>
-      <c r="K18" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="M18" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-    </row>
-    <row r="22" spans="1:13" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -3163,7 +3452,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
+      <c r="J24" s="70"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
@@ -3490,16 +3779,63 @@
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
     </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A14:A21"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="D2:D7"/>
     <mergeCell ref="E2:E7"/>
     <mergeCell ref="F2:F7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
+  <conditionalFormatting sqref="M2:M689">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="done">
+      <formula>NOT(ISERROR(SEARCH("done",M2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3509,7 +3845,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3524,391 +3860,391 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="54" t="s">
-        <v>102</v>
-      </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="38"/>
+      <c r="A1" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="54"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="28"/>
     </row>
     <row r="2" spans="1:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="38"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="42"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="28"/>
     </row>
     <row r="3" spans="1:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="36">
         <v>9</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="33">
         <v>9</v>
       </c>
-      <c r="D3" s="50">
+      <c r="D3" s="37">
         <v>6</v>
       </c>
-      <c r="E3" s="49">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!E$2))</f>
-        <v>6</v>
-      </c>
-      <c r="F3" s="43">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!F$2))</f>
+      <c r="E3" s="36">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!E$2))</f>
+        <v>9</v>
+      </c>
+      <c r="F3" s="33">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!F$2))</f>
         <v>0</v>
       </c>
-      <c r="G3" s="50">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!G$2))</f>
+      <c r="G3" s="37">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!G$2))</f>
         <v>0</v>
       </c>
-      <c r="H3" s="49">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!H$2))</f>
+      <c r="H3" s="36">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!H$2))</f>
         <v>0</v>
       </c>
-      <c r="I3" s="43">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!I$2))</f>
+      <c r="I3" s="33">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!I$2))</f>
         <v>0</v>
       </c>
-      <c r="J3" s="50">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!J$2))</f>
+      <c r="J3" s="37">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A3,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!J$2))</f>
         <v>0</v>
       </c>
-      <c r="K3" s="36">
+      <c r="K3" s="26">
         <f t="shared" ref="K3:K8" si="0">SUM(B3:D3)-SUM(H3:J3)</f>
         <v>24</v>
       </c>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="49">
+      <c r="A4" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="36">
         <v>9</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="33">
         <v>9</v>
       </c>
-      <c r="D4" s="50">
+      <c r="D4" s="37">
         <v>6</v>
       </c>
-      <c r="E4" s="49">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!E$2))</f>
-        <v>12</v>
-      </c>
-      <c r="F4" s="43">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!F$2))</f>
+      <c r="E4" s="36">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!E$2))</f>
+        <v>9</v>
+      </c>
+      <c r="F4" s="33">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!F$2))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="50">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!G$2))</f>
+      <c r="G4" s="37">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!G$2))</f>
         <v>0</v>
       </c>
-      <c r="H4" s="49">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!H$2))</f>
+      <c r="H4" s="36">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!H$2))</f>
+        <v>4</v>
+      </c>
+      <c r="I4" s="33">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!I$2))</f>
         <v>0</v>
       </c>
-      <c r="I4" s="43">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!I$2))</f>
+      <c r="J4" s="37">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!J$2))</f>
         <v>0</v>
       </c>
-      <c r="J4" s="50">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A4,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!J$2))</f>
+      <c r="K4" s="26">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+    </row>
+    <row r="5" spans="1:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="36">
+        <v>9</v>
+      </c>
+      <c r="C5" s="33">
+        <v>9</v>
+      </c>
+      <c r="D5" s="37">
+        <v>6</v>
+      </c>
+      <c r="E5" s="36">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!E$2))</f>
+        <v>9</v>
+      </c>
+      <c r="F5" s="33">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!F$2))</f>
         <v>0</v>
       </c>
-      <c r="K4" s="36">
+      <c r="G5" s="37">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!G$2))</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="36">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!H$2))</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="33">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!I$2))</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="37">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!J$2))</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="26">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-    </row>
-    <row r="5" spans="1:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="49">
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+    </row>
+    <row r="6" spans="1:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="36">
         <v>9</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C6" s="33">
         <v>9</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D6" s="37">
         <v>6</v>
       </c>
-      <c r="E5" s="49">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!E$2))</f>
-        <v>8</v>
-      </c>
-      <c r="F5" s="43">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!F$2))</f>
+      <c r="E6" s="36">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!E$2))</f>
+        <v>9</v>
+      </c>
+      <c r="F6" s="33">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!F$2))</f>
         <v>0</v>
       </c>
-      <c r="G5" s="50">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!G$2))</f>
+      <c r="G6" s="37">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!G$2))</f>
         <v>0</v>
       </c>
-      <c r="H5" s="49">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!H$2))</f>
+      <c r="H6" s="36">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!H$2))</f>
         <v>0</v>
       </c>
-      <c r="I5" s="43">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!I$2))</f>
+      <c r="I6" s="33">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!I$2))</f>
         <v>0</v>
       </c>
-      <c r="J5" s="50">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A5,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!J$2))</f>
+      <c r="J6" s="37">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!J$2))</f>
         <v>0</v>
       </c>
-      <c r="K5" s="36">
+      <c r="K6" s="26">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-    </row>
-    <row r="6" spans="1:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="49">
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+    </row>
+    <row r="7" spans="1:14" ht="22" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="36">
         <v>9</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C7" s="33">
         <v>9</v>
       </c>
-      <c r="D6" s="50">
+      <c r="D7" s="37">
         <v>6</v>
       </c>
-      <c r="E6" s="49">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!E$2))</f>
-        <v>6</v>
-      </c>
-      <c r="F6" s="43">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!F$2))</f>
+      <c r="E7" s="36">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!E$2))</f>
+        <v>9</v>
+      </c>
+      <c r="F7" s="33">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!F$2))</f>
         <v>0</v>
       </c>
-      <c r="G6" s="50">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!G$2))</f>
+      <c r="G7" s="37">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!G$2))</f>
         <v>0</v>
       </c>
-      <c r="H6" s="49">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!H$2))</f>
+      <c r="H7" s="36">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!H$2))</f>
         <v>0</v>
       </c>
-      <c r="I6" s="43">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!I$2))</f>
+      <c r="I7" s="33">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!I$2))</f>
         <v>0</v>
       </c>
-      <c r="J6" s="50">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A6,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!J$2))</f>
+      <c r="J7" s="37">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!J$2))</f>
         <v>0</v>
       </c>
-      <c r="K6" s="36">
+      <c r="K7" s="26">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-    </row>
-    <row r="7" spans="1:14" ht="22" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="49">
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+    </row>
+    <row r="8" spans="1:14" ht="23" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="38">
         <v>9</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C8" s="39">
         <v>9</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D8" s="40">
         <v>6</v>
       </c>
-      <c r="E7" s="49">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!E$2))</f>
-        <v>8</v>
-      </c>
-      <c r="F7" s="43">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!F$2))</f>
+      <c r="E8" s="38">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!E$2))</f>
+        <v>9</v>
+      </c>
+      <c r="F8" s="39">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!F$2))</f>
         <v>0</v>
       </c>
-      <c r="G7" s="50">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!G$2))</f>
+      <c r="G8" s="40">
+        <f>SUMIFS('Sprint Backlog'!$J$2:$J$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!G$2))</f>
         <v>0</v>
       </c>
-      <c r="H7" s="49">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!H$2))</f>
+      <c r="H8" s="38">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!H$2))</f>
         <v>0</v>
       </c>
-      <c r="I7" s="43">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!I$2))</f>
+      <c r="I8" s="39">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!I$2))</f>
         <v>0</v>
       </c>
-      <c r="J7" s="50">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A7,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!J$2))</f>
+      <c r="J8" s="40">
+        <f>SUMIFS('Sprint Backlog'!$L$2:$L$21,'Sprint Backlog'!$G$2:$G$21,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$21,RIGHT(Auslastung!J$2))</f>
         <v>0</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K8" s="27">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-    </row>
-    <row r="8" spans="1:14" ht="23" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="51">
-        <v>9</v>
-      </c>
-      <c r="C8" s="52">
-        <v>9</v>
-      </c>
-      <c r="D8" s="53">
-        <v>6</v>
-      </c>
-      <c r="E8" s="51">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!E$2))</f>
-        <v>10</v>
-      </c>
-      <c r="F8" s="52">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!F$2))</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="53">
-        <f>SUMIFS('Sprint Backlog'!$J$2:$J$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!G$2))</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="51">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!H$2))</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="52">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!I$2))</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="53">
-        <f>SUMIFS('Sprint Backlog'!$L$2:$L$18,'Sprint Backlog'!$G$2:$G$18,Auslastung!$A8,'Sprint Backlog'!$C$2:$C$18,RIGHT(Auslastung!J$2))</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="37">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
     </row>
     <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
     </row>
     <row r="10" spans="1:14" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="56">
+      <c r="A10" s="22"/>
+      <c r="B10" s="43">
         <f>SUM(B3:B8)</f>
         <v>54</v>
       </c>
-      <c r="C10" s="56">
+      <c r="C10" s="43">
         <f t="shared" ref="C10:K10" si="1">SUM(C3:C8)</f>
         <v>54</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="43">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="43">
         <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="F10" s="56">
+        <v>54</v>
+      </c>
+      <c r="F10" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="56">
+      <c r="G10" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="56">
+      <c r="H10" s="43">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I10" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="56">
+      <c r="J10" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="56">
+      <c r="K10" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="33">
-        <f t="shared" si="1"/>
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -3919,20 +4255,23 @@
     <mergeCell ref="H1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K8">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>